<commit_message>
major agent mobility bug fix
</commit_message>
<xml_diff>
--- a/Input Files/Micropolis_pop_at_node_kind.xlsx
+++ b/Input Files/Micropolis_pop_at_node_kind.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\squar\Documents\hydraulic_ABM\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165F0B22-7B01-48F7-B468-BFB22A1BC301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22315A4-2DD5-47E0-B294-4C1212B63516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25860" yWindow="-960" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="2715" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,9 +381,10 @@
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
       </c>
@@ -424,9 +425,8 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -447,9 +447,8 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -470,9 +469,8 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -493,9 +491,8 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -516,9 +513,8 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -529,19 +525,19 @@
         <v>39</v>
       </c>
       <c r="D7">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="E7">
-        <v>3148</v>
+        <v>3163</v>
       </c>
       <c r="F7">
         <v>4605</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -552,19 +548,19 @@
         <v>54</v>
       </c>
       <c r="D8">
-        <v>612</v>
+        <v>585</v>
       </c>
       <c r="E8">
-        <v>2848</v>
+        <v>2875</v>
       </c>
       <c r="F8">
         <v>4606</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -575,19 +571,19 @@
         <v>59</v>
       </c>
       <c r="D9">
-        <v>1095</v>
+        <v>1046</v>
       </c>
       <c r="E9">
-        <v>2360</v>
+        <v>2409</v>
       </c>
       <c r="F9">
         <v>4606</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -598,19 +594,19 @@
         <v>54</v>
       </c>
       <c r="D10">
-        <v>1555</v>
+        <v>1486</v>
       </c>
       <c r="E10">
-        <v>1905</v>
+        <v>1974</v>
       </c>
       <c r="F10">
         <v>4606</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -621,19 +617,19 @@
         <v>49</v>
       </c>
       <c r="D11">
-        <v>1946</v>
+        <v>1860</v>
       </c>
       <c r="E11">
-        <v>1519</v>
+        <v>1605</v>
       </c>
       <c r="F11">
         <v>4606</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -644,19 +640,19 @@
         <v>59</v>
       </c>
       <c r="D12">
-        <v>2098</v>
+        <v>1916</v>
       </c>
       <c r="E12">
-        <v>1357</v>
+        <v>1539</v>
       </c>
       <c r="F12">
         <v>4606</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -667,19 +663,19 @@
         <v>108</v>
       </c>
       <c r="D13">
-        <v>2148</v>
+        <v>2053</v>
       </c>
       <c r="E13">
-        <v>1258</v>
+        <v>1353</v>
       </c>
       <c r="F13">
         <v>4606</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -690,19 +686,19 @@
         <v>103</v>
       </c>
       <c r="D14">
-        <v>2152</v>
+        <v>2057</v>
       </c>
       <c r="E14">
-        <v>1259</v>
+        <v>1354</v>
       </c>
       <c r="F14">
         <v>4606</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -713,19 +709,19 @@
         <v>88</v>
       </c>
       <c r="D15">
-        <v>2164</v>
+        <v>2068</v>
       </c>
       <c r="E15">
-        <v>1262</v>
+        <v>1358</v>
       </c>
       <c r="F15">
         <v>4606</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -736,19 +732,19 @@
         <v>83</v>
       </c>
       <c r="D16">
-        <v>2118</v>
+        <v>2024</v>
       </c>
       <c r="E16">
-        <v>1313</v>
+        <v>1407</v>
       </c>
       <c r="F16">
         <v>4606</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -759,19 +755,19 @@
         <v>79</v>
       </c>
       <c r="D17">
-        <v>2032</v>
+        <v>1942</v>
       </c>
       <c r="E17">
-        <v>1403</v>
+        <v>1493</v>
       </c>
       <c r="F17">
         <v>4606</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -782,19 +778,19 @@
         <v>83</v>
       </c>
       <c r="D18">
-        <v>1870</v>
+        <v>1787</v>
       </c>
       <c r="E18">
-        <v>1561</v>
+        <v>1644</v>
       </c>
       <c r="F18">
         <v>4606</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -805,19 +801,19 @@
         <v>88</v>
       </c>
       <c r="D19">
-        <v>1528</v>
+        <v>1460</v>
       </c>
       <c r="E19">
-        <v>1898</v>
+        <v>1966</v>
       </c>
       <c r="F19">
         <v>4606</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -828,19 +824,19 @@
         <v>108</v>
       </c>
       <c r="D20">
-        <v>1065</v>
+        <v>1018</v>
       </c>
       <c r="E20">
-        <v>2341</v>
+        <v>2388</v>
       </c>
       <c r="F20">
         <v>4606</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -851,19 +847,19 @@
         <v>108</v>
       </c>
       <c r="D21">
-        <v>639</v>
+        <v>611</v>
       </c>
       <c r="E21">
-        <v>2767</v>
+        <v>2795</v>
       </c>
       <c r="F21">
         <v>4606</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8</v>
       </c>
@@ -874,19 +870,19 @@
         <v>88</v>
       </c>
       <c r="D22">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="E22">
-        <v>3099</v>
+        <v>3114</v>
       </c>
       <c r="F22">
         <v>4606</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -907,9 +903,8 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -930,9 +925,8 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
@@ -953,7 +947,6 @@
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>